<commit_message>
adds column to spreadsheet for today if none exists already, writes ozeret name in second row in that column
</commit_message>
<xml_diff>
--- a/resources/files/test2.xlsx
+++ b/resources/files/test2.xlsx
@@ -413,12 +413,13 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="27.05078125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.05078125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.83984375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -459,6 +460,9 @@
       </c>
       <c r="D3">
         <v>3</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
changed three buttons into one button, added save and save and quit buttons, added functionality to all buttons. ready for testing
</commit_message>
<xml_diff>
--- a/resources/files/test2.xlsx
+++ b/resources/files/test2.xlsx
@@ -74,22 +74,22 @@
     <t>B6</t>
   </si>
   <si>
+    <t>LONGNAME</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>ReallyLongName WithALastName</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
     <t>B7</t>
   </si>
   <si>
     <t>B8</t>
-  </si>
-  <si>
-    <t>LONGNAME</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>ReallyLongName WithALastName</t>
-  </si>
-  <si>
-    <t>Last Name</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -494,7 +494,7 @@
         <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
@@ -502,23 +502,23 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>